<commit_message>
final commit 3.0 ```
</commit_message>
<xml_diff>
--- a/Anagrafica.xlsx
+++ b/Anagrafica.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t xml:space="preserve">mario rossi lavora in banca </t>
   </si>
@@ -71,16 +71,16 @@
     <t>RSSMRA80A01F205X</t>
   </si>
   <si>
-    <t>Divorziato</t>
+    <t>Coniugato</t>
   </si>
   <si>
     <t>Milano</t>
   </si>
   <si>
-    <t>Laurea in Medicina</t>
-  </si>
-  <si>
-    <t>Medico</t>
+    <t>Laurea magistrale in Economia</t>
+  </si>
+  <si>
+    <t>Direttore di banca</t>
   </si>
   <si>
     <t>Filippo</t>
@@ -92,13 +92,13 @@
     <t>FLPBCH77A01F205K</t>
   </si>
   <si>
-    <t>Sposato</t>
-  </si>
-  <si>
-    <t>Laurea in Economia</t>
-  </si>
-  <si>
-    <t>Contabile</t>
+    <t>Celibe</t>
+  </si>
+  <si>
+    <t>Licenza media</t>
+  </si>
+  <si>
+    <t>Barista</t>
   </si>
   <si>
     <t>Giuseppina</t>
@@ -110,37 +110,34 @@
     <t>CFRGPP65A41A662P</t>
   </si>
   <si>
-    <t>Nubile</t>
+    <t>Coniugata</t>
   </si>
   <si>
     <t>Bari</t>
   </si>
   <si>
-    <t>Diploma di maturita'</t>
-  </si>
-  <si>
-    <t>Insegnante</t>
-  </si>
-  <si>
-    <t>Vincenzo</t>
-  </si>
-  <si>
-    <t>Verdi</t>
+    <t>Laurea magistrale in Giurisprudenza</t>
+  </si>
+  <si>
+    <t>Avvocato</t>
+  </si>
+  <si>
+    <t>Giovanni</t>
+  </si>
+  <si>
+    <t>Mele</t>
   </si>
   <si>
     <t>MLEGNN97A01D150L</t>
   </si>
   <si>
-    <t>Celibe</t>
-  </si>
-  <si>
     <t>Cremona</t>
   </si>
   <si>
-    <t>Laurea magistrale in Economia</t>
-  </si>
-  <si>
-    <t>Imprenditore settore investimenti</t>
+    <t>Laurea triennale in Informatica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulente </t>
   </si>
 </sst>
 </file>
@@ -158,13 +155,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -196,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -207,10 +204,16 @@
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -529,17 +532,17 @@
   <cols>
     <col min="1" max="1" style="2" width="10.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="2" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="15.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="2" width="20.433571428571426" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="14.862142857142858" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="13.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="30.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="20.433571428571426" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="2" width="31.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="29.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="18.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -578,8 +581,8 @@
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3">
-        <v>25204</v>
+      <c r="C2" s="6">
+        <v>29221</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -591,10 +594,10 @@
         <v>18</v>
       </c>
       <c r="G2" s="5">
+        <v>2</v>
+      </c>
+      <c r="H2" s="7">
         <v>3</v>
-      </c>
-      <c r="H2" s="5">
-        <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>19</v>
@@ -610,8 +613,8 @@
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3">
-        <v>33604</v>
+      <c r="C3" s="6">
+        <v>28126</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>23</v>
@@ -623,10 +626,10 @@
         <v>18</v>
       </c>
       <c r="G3" s="5">
-        <v>3</v>
-      </c>
-      <c r="H3" s="5">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>25</v>
@@ -642,8 +645,8 @@
       <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="3">
-        <v>32143</v>
+      <c r="C4" s="6">
+        <v>23743</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>29</v>
@@ -657,7 +660,7 @@
       <c r="G4" s="5">
         <v>2</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="7">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -674,29 +677,29 @@
       <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="3">
-        <v>25569</v>
+      <c r="C5" s="6">
+        <v>35431</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="7">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>